<commit_message>
Change mapping of the different parts in Mobility from .value to .component, because There Can Only Be One in .value
</commit_message>
<xml_diff>
--- a/Mappings/Mobility - STU3.xlsx
+++ b/Mappings/Mobility - STU3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1283B19B-06AE-47A7-BBD7-78C8FFE59308}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7202FD3-358C-450A-A488-7527D47B3705}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -647,21 +647,6 @@
     <t>.comment</t>
   </si>
   <si>
-    <t>.valueCodeableConcept, slice "climbingStairs"</t>
-  </si>
-  <si>
-    <t>.valueCodeableConcept, slice "changingPosition"</t>
-  </si>
-  <si>
-    <t>.valueCodeableConcept, slice "maintainingPosition"</t>
-  </si>
-  <si>
-    <t>.valueCodeableConcept, slice "transfer"</t>
-  </si>
-  <si>
-    <t>.valueCodeableConcept, slice "walking"</t>
-  </si>
-  <si>
     <t>.medicalDevice, MedicalDevice extension (http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)</t>
   </si>
   <si>
@@ -669,6 +654,21 @@
   </si>
   <si>
     <t>equal</t>
+  </si>
+  <si>
+    <t>.component, slice "walking"</t>
+  </si>
+  <si>
+    <t>.component, slice "climbingStairs"</t>
+  </si>
+  <si>
+    <t>.component, slice "changingPosition"</t>
+  </si>
+  <si>
+    <t>.component, slice "maintainingPosition"</t>
+  </si>
+  <si>
+    <t>.component, slice "transfer"</t>
   </si>
 </sst>
 </file>
@@ -850,9 +850,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -862,6 +859,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1136,9 +1136,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1154,7 +1154,7 @@
                   <a14:compatExt spid="_x0000_s11265"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB64F3CB-87C2-42B1-A435-3134856CD769}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000012C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1203,9 +1203,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1221,7 +1221,7 @@
                   <a14:compatExt spid="_x0000_s11266"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AECC2DE6-77BC-4853-874A-E8FB21B52195}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000022C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1270,9 +1270,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1288,7 +1288,7 @@
                   <a14:compatExt spid="_x0000_s11267"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5833124-7ABC-4F35-BFAE-4ECFC510810C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000032C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1337,9 +1337,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1355,7 +1355,7 @@
                   <a14:compatExt spid="_x0000_s11268"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{677E28E7-131B-406E-AE94-27E7AA910778}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000042C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1404,9 +1404,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1422,7 +1422,7 @@
                   <a14:compatExt spid="_x0000_s11269"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E4DC09C-E85E-40CD-8256-B3F60CAA5E86}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000052C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1471,9 +1471,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1489,7 +1489,7 @@
                   <a14:compatExt spid="_x0000_s11270"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74C76191-39AD-4FBA-A8DC-7577FC2F2288}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000062C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1538,9 +1538,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1556,7 +1556,7 @@
                   <a14:compatExt spid="_x0000_s11271"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2836EDD-245E-4CBA-BE68-9871E27CFED1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000072C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1605,9 +1605,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1623,7 +1623,7 @@
                   <a14:compatExt spid="_x0000_s11272"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1F477BE-DCE7-467E-AB0A-DB344497B261}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000082C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1672,9 +1672,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1690,7 +1690,7 @@
                   <a14:compatExt spid="_x0000_s11273"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9998C10-F88A-4C40-B00E-95FB078E8E31}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000092C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1739,9 +1739,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1757,7 +1757,7 @@
                   <a14:compatExt spid="_x0000_s11274"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{976720C3-408A-4B4E-B6F2-24C98C1BE920}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1806,9 +1806,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1824,7 +1824,7 @@
                   <a14:compatExt spid="_x0000_s11275"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C152780-E9E0-478A-9B24-5B362FA76A0B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1873,9 +1873,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1891,7 +1891,7 @@
                   <a14:compatExt spid="_x0000_s11276"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6D04AD0-FE04-40FE-A0F0-79D3ADB984CA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1940,9 +1940,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -1958,7 +1958,7 @@
                   <a14:compatExt spid="_x0000_s11277"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27F4E33B-98D7-4A0C-8875-86CB0CE1226E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2007,9 +2007,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -2025,7 +2025,7 @@
                   <a14:compatExt spid="_x0000_s11278"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E8EC330-6A99-4B00-B07C-1CF0E9B09163}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2074,9 +2074,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -2092,7 +2092,7 @@
                   <a14:compatExt spid="_x0000_s11279"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76251533-7E2C-4267-ADA8-A1223B1972AF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2141,9 +2141,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -2159,7 +2159,7 @@
                   <a14:compatExt spid="_x0000_s11280"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F1AF06D-5B7B-4D6E-8091-2ECC09108099}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000102C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2208,9 +2208,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -2226,7 +2226,7 @@
                   <a14:compatExt spid="_x0000_s11281"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D64C84C-64B8-4D4B-973C-17E02469156D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000112C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2275,9 +2275,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -2293,7 +2293,7 @@
                   <a14:compatExt spid="_x0000_s11282"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FE00F6D-39B8-4A63-A8F6-D29F2A801BFD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000122C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2342,15 +2342,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>20955</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2360,7 +2360,7 @@
                   <a14:compatExt spid="_x0000_s11283"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27C0AE04-6D74-4F1E-AE0B-648E18ACE2C0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000132C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2409,15 +2409,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>20955</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2427,7 +2427,7 @@
                   <a14:compatExt spid="_x0000_s11284"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2EC4C38-F643-431D-9FC6-13AD08FA3A59}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000142C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2476,9 +2476,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>49530</xdr:colOff>
+          <xdr:colOff>57150</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>129540</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -2494,7 +2494,7 @@
                   <a14:compatExt spid="_x0000_s11285"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{390E006F-E52C-48B3-913F-5C61F7764175}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000152C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2543,9 +2543,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>49530</xdr:colOff>
+          <xdr:colOff>57150</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>129540</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -2561,7 +2561,7 @@
                   <a14:compatExt spid="_x0000_s11286"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCA3D924-4013-4468-A7C4-FF034F21FB48}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000162C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2610,9 +2610,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -2628,7 +2628,7 @@
                   <a14:compatExt spid="_x0000_s11287"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDEC222E-1AE6-4CDD-B419-C823C8C8780C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000172C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2677,9 +2677,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -2695,7 +2695,7 @@
                   <a14:compatExt spid="_x0000_s11288"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3F28C97-C07E-4745-94A2-CB4D588093C1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000182C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2741,14 +2741,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="828675" cy="230505"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11289" name="Check Box 25" hidden="1">
@@ -2757,7 +2762,7 @@
                   <a14:compatExt spid="_x0000_s11289"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{227CAEAF-EAD8-4E60-9D7D-18B964C42C16}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000192C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2797,20 +2802,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="828675" cy="230505"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11290" name="Check Box 26" hidden="1">
@@ -2819,7 +2829,7 @@
                   <a14:compatExt spid="_x0000_s11290"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{179A8677-18BB-4A3F-B651-96E2B36485F6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001A2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2859,20 +2869,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>49530</xdr:colOff>
+          <xdr:colOff>57150</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>129540</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="822960" cy="228600"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11291" name="Check Box 27" hidden="1">
@@ -2881,7 +2896,7 @@
                   <a14:compatExt spid="_x0000_s11291"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C0A69A2-DBF1-4605-BC58-DABB02873580}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001B2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2921,20 +2936,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>49530</xdr:colOff>
+          <xdr:colOff>57150</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>129540</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="822960" cy="228600"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11292" name="Check Box 28" hidden="1">
@@ -2943,7 +2963,7 @@
                   <a14:compatExt spid="_x0000_s11292"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05CBF375-A301-4F13-B9FE-4938A867373F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001C2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2983,20 +3003,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="828675" cy="228600"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11293" name="Check Box 29" hidden="1">
@@ -3005,7 +3030,7 @@
                   <a14:compatExt spid="_x0000_s11293"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EF93987-9F55-4566-A37A-F3478C9C067E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001D2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3045,20 +3070,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="828675" cy="228600"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11294" name="Check Box 30" hidden="1">
@@ -3067,7 +3097,7 @@
                   <a14:compatExt spid="_x0000_s11294"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2E79817-D211-43C7-8B6C-05329EBD7CF6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001E2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3107,7 +3137,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -3415,13 +3445,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3429,7 +3459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3437,7 +3467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3445,7 +3475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3453,7 +3483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -3461,7 +3491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3469,7 +3499,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -3477,7 +3507,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3485,7 +3515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -3493,7 +3523,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -3501,7 +3531,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
@@ -3509,7 +3539,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>57</v>
       </c>
@@ -3517,7 +3547,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>59</v>
       </c>
@@ -3543,7 +3573,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -3552,18 +3582,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>124</v>
       </c>
@@ -3580,7 +3610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>161</v>
       </c>
@@ -3597,7 +3627,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>163</v>
       </c>
@@ -3614,7 +3644,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>165</v>
       </c>
@@ -3649,37 +3679,37 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>172</v>
       </c>
@@ -3695,19 +3725,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="15"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -3715,7 +3745,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -3723,7 +3753,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -3731,7 +3761,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -3739,7 +3769,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -3747,7 +3777,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
@@ -3755,13 +3785,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3769,13 +3799,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -3783,13 +3813,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
@@ -3797,7 +3827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
@@ -3805,7 +3835,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
@@ -3813,7 +3843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
@@ -3821,7 +3851,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
@@ -3829,7 +3859,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -3837,7 +3867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -3845,7 +3875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -3853,7 +3883,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>49</v>
       </c>
@@ -3861,7 +3891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
@@ -3869,7 +3899,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
@@ -3877,7 +3907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>53</v>
       </c>
@@ -3902,9 +3932,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
@@ -3921,117 +3951,117 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="O1" s="16"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="O1" s="15"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C10" s="18" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C10" s="17" t="s">
         <v>193</v>
       </c>
       <c r="D10" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4050,15 +4080,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4072,15 +4102,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4094,15 +4124,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4116,15 +4146,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4138,15 +4168,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4160,15 +4190,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4182,15 +4212,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4204,15 +4234,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4226,15 +4256,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4248,15 +4278,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4270,15 +4300,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4292,15 +4322,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4314,15 +4344,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4336,15 +4366,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4358,15 +4388,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4380,15 +4410,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4402,15 +4432,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4424,15 +4454,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4446,15 +4476,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4468,15 +4498,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4490,15 +4520,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>53340</xdr:colOff>
+                    <xdr:colOff>57150</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>129540</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4512,15 +4542,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>53340</xdr:colOff>
+                    <xdr:colOff>57150</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>129540</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4534,15 +4564,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4556,15 +4586,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4578,15 +4608,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4600,15 +4630,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4622,15 +4652,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>53340</xdr:colOff>
+                    <xdr:colOff>57150</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>129540</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4644,15 +4674,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>53340</xdr:colOff>
+                    <xdr:colOff>57150</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>129540</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4666,15 +4696,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4688,15 +4718,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4713,11 +4743,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -4728,13 +4758,13 @@
     <col min="13" max="13" width="75" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" customWidth="1"/>
-    <col min="17" max="17" width="20.88671875" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
-    <col min="20" max="20" width="47.44140625" customWidth="1"/>
+    <col min="20" max="20" width="47.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>55</v>
       </c>
@@ -4783,7 +4813,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>70</v>
       </c>
@@ -4820,7 +4850,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="2:20" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>76</v>
@@ -4847,25 +4877,25 @@
       <c r="M4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="19" t="s">
         <v>83</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>84</v>
       </c>
       <c r="P4" s="2"/>
-      <c r="Q4" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="S4" s="20" t="s">
+      <c r="Q4" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="S4" s="19" t="s">
         <v>2</v>
       </c>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="2:20" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>85</v>
@@ -4899,18 +4929,18 @@
         <v>90</v>
       </c>
       <c r="P5" s="2"/>
-      <c r="Q5" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="R5" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="S5" s="20" t="s">
+      <c r="Q5" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="S5" s="19" t="s">
         <v>2</v>
       </c>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="2:20" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>91</v>
@@ -4944,18 +4974,18 @@
         <v>96</v>
       </c>
       <c r="P6" s="2"/>
-      <c r="Q6" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="R6" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="S6" s="20" t="s">
+      <c r="Q6" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="S6" s="19" t="s">
         <v>2</v>
       </c>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="2:20" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
         <v>97</v>
@@ -4989,18 +5019,18 @@
         <v>102</v>
       </c>
       <c r="P7" s="2"/>
-      <c r="Q7" s="20" t="s">
+      <c r="Q7" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="R7" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="R7" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="S7" s="20" t="s">
+      <c r="S7" s="19" t="s">
         <v>2</v>
       </c>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="2:20" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
         <v>103</v>
@@ -5034,18 +5064,18 @@
         <v>108</v>
       </c>
       <c r="P8" s="2"/>
-      <c r="Q8" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="R8" s="20" t="s">
+      <c r="Q8" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="S8" s="20" t="s">
+      <c r="R8" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="S8" s="19" t="s">
         <v>2</v>
       </c>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="2:20" ht="69" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:20" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
         <v>109</v>
@@ -5077,16 +5107,16 @@
         <v>116</v>
       </c>
       <c r="P9" s="2"/>
-      <c r="Q9" s="20" t="s">
-        <v>209</v>
+      <c r="Q9" s="19" t="s">
+        <v>204</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
-      <c r="T9" s="20" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="T9" s="19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
         <v>117</v>
@@ -5118,7 +5148,7 @@
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
-      <c r="Q10" s="20" t="s">
+      <c r="Q10" s="19" t="s">
         <v>203</v>
       </c>
       <c r="R10" s="2"/>
@@ -5148,7 +5178,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5157,18 +5187,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>124</v>
       </c>
@@ -5185,7 +5215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>128</v>
       </c>
@@ -5202,7 +5232,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>133</v>
       </c>
@@ -5219,7 +5249,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>136</v>
       </c>
@@ -5254,7 +5284,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5263,18 +5293,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>124</v>
       </c>
@@ -5291,7 +5321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>140</v>
       </c>
@@ -5308,7 +5338,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>142</v>
       </c>
@@ -5325,7 +5355,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>144</v>
       </c>
@@ -5360,7 +5390,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5369,18 +5399,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>124</v>
       </c>
@@ -5397,7 +5427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>147</v>
       </c>
@@ -5414,7 +5444,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>149</v>
       </c>
@@ -5431,7 +5461,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>151</v>
       </c>
@@ -5466,7 +5496,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5475,18 +5505,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>124</v>
       </c>
@@ -5503,7 +5533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>154</v>
       </c>
@@ -5520,7 +5550,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>156</v>
       </c>
@@ -5537,7 +5567,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>158</v>
       </c>

</xml_diff>